<commit_message>
Questionid input directly reading from Content output
</commit_message>
<xml_diff>
--- a/Automation-UserCMD/TestData/Outputs/AssetSkillMappingOutput.xlsx
+++ b/Automation-UserCMD/TestData/Outputs/AssetSkillMappingOutput.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssetSkillsMapping (2)" sheetId="1" r:id="Re4b0cd21239e4b8c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AssetSkillsMapping (2)" sheetId="1" r:id="R3944df2dd4c14b1c"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -1632,6 +1632,2114 @@
         <x:v>no</x:v>
       </x:c>
     </x:row>
+    <x:row r="96">
+      <x:c r="A96" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B96" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba8ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="C96" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D96" t="str">
+        <x:v>8ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="E96" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97">
+      <x:c r="A97" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B97" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba8ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="C97" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D97" t="str">
+        <x:v> </x:v>
+      </x:c>
+      <x:c r="E97" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98">
+      <x:c r="A98" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B98" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bae5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="C98" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D98" t="str">
+        <x:v>e5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="E98" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99">
+      <x:c r="A99" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B99" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba36dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="C99" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D99" t="str">
+        <x:v>36dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="E99" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100">
+      <x:c r="A100" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B100" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba1e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="C100" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D100" t="str">
+        <x:v>1e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="E100" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101">
+      <x:c r="A101" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B101" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba29b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="C101" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D101" t="str">
+        <x:v>29b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="E101" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102">
+      <x:c r="A102" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B102" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba29b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="C102" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D102" t="str">
+        <x:v>29b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="E102" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103">
+      <x:c r="A103" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B103" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba75357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="C103" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D103" t="str">
+        <x:v>75357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="E103" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104">
+      <x:c r="A104" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B104" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba9be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="C104" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D104" t="str">
+        <x:v>9be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="E104" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105">
+      <x:c r="A105" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B105" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba9be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="C105" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D105" t="str">
+        <x:v>9be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="E105" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106">
+      <x:c r="A106" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B106" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bae5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="C106" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D106" t="str">
+        <x:v>e5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="E106" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107">
+      <x:c r="A107" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B107" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba8ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="C107" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D107" t="str">
+        <x:v>8ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="E107" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108">
+      <x:c r="A108" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B108" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba8ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="C108" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D108" t="str">
+        <x:v>8ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="E108" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109">
+      <x:c r="A109" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B109" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658baa6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="C109" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D109" t="str">
+        <x:v>a6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="E109" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110">
+      <x:c r="A110" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B110" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba46f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="C110" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D110" t="str">
+        <x:v>46f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="E110" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111">
+      <x:c r="A111" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B111" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba46f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="C111" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D111" t="str">
+        <x:v>46f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="E111" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112">
+      <x:c r="A112" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B112" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba5b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="C112" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D112" t="str">
+        <x:v>5b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="E112" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113">
+      <x:c r="A113" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B113" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba5b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="C113" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D113" t="str">
+        <x:v>5b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="E113" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114">
+      <x:c r="A114" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B114" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba0d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="C114" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D114" t="str">
+        <x:v>0d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="E114" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="115">
+      <x:c r="A115" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B115" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="C115" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D115" t="str">
+        <x:v>761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="E115" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116">
+      <x:c r="A116" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B116" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658baf0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="C116" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D116" t="str">
+        <x:v>f0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="E116" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117">
+      <x:c r="A117" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B117" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658baf0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="C117" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D117" t="str">
+        <x:v>f0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="E117" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118">
+      <x:c r="A118" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B118" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba36dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="C118" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D118" t="str">
+        <x:v>36dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="E118" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119">
+      <x:c r="A119" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B119" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba1e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="C119" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D119" t="str">
+        <x:v>1e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="E119" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120">
+      <x:c r="A120" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B120" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba75357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="C120" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D120" t="str">
+        <x:v>75357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="E120" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121">
+      <x:c r="A121" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B121" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658baa294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="C121" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D121" t="str">
+        <x:v>a294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="E121" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="122">
+      <x:c r="A122" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B122" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658baa294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="C122" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D122" t="str">
+        <x:v>a294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="E122" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="123">
+      <x:c r="A123" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B123" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bab4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="C123" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D123" t="str">
+        <x:v>b4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="E123" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="124">
+      <x:c r="A124" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B124" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658baa6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="C124" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D124" t="str">
+        <x:v>a6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="E124" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="125">
+      <x:c r="A125" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B125" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba4c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="C125" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D125" t="str">
+        <x:v>4c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="E125" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="126">
+      <x:c r="A126" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B126" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba4c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="C126" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D126" t="str">
+        <x:v>4c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="E126" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="127">
+      <x:c r="A127" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B127" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba52022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="C127" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D127" t="str">
+        <x:v>52022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="E127" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="128">
+      <x:c r="A128" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B128" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bad5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="C128" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D128" t="str">
+        <x:v>d5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="E128" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="129">
+      <x:c r="A129" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B129" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bad5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="C129" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D129" t="str">
+        <x:v>d5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="E129" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="130">
+      <x:c r="A130" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B130" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658badcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="C130" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D130" t="str">
+        <x:v>dcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="E130" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="131">
+      <x:c r="A131" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B131" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658badcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="C131" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D131" t="str">
+        <x:v>dcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="E131" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="132">
+      <x:c r="A132" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B132" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658badeb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="C132" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D132" t="str">
+        <x:v>deb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="E132" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="133">
+      <x:c r="A133" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B133" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba3a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="C133" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D133" t="str">
+        <x:v>3a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="E133" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="134">
+      <x:c r="A134" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B134" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba31bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="C134" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D134" t="str">
+        <x:v>31bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="E134" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="135">
+      <x:c r="A135" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B135" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba31bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="C135" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D135" t="str">
+        <x:v>31bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="E135" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="136">
+      <x:c r="A136" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B136" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="C136" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D136" t="str">
+        <x:v>416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="E136" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="137">
+      <x:c r="A137" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B137" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba9237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="C137" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D137" t="str">
+        <x:v>9237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="E137" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="138">
+      <x:c r="A138" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B138" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba9237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="C138" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D138" t="str">
+        <x:v>9237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="E138" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139">
+      <x:c r="A139" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B139" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba3b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="C139" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D139" t="str">
+        <x:v>3b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="E139" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140">
+      <x:c r="A140" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B140" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba3b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="C140" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D140" t="str">
+        <x:v>3b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="E140" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="141">
+      <x:c r="A141" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B141" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bae1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="C141" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D141" t="str">
+        <x:v>e1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="E141" t="str">
+        <x:v>yes</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="142">
+      <x:c r="A142" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B142" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bae1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="C142" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D142" t="str">
+        <x:v>e1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="E142" t="str">
+        <x:v>yes</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="143">
+      <x:c r="A143" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B143" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba0d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="C143" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D143" t="str">
+        <x:v>0d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="E143" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="144">
+      <x:c r="A144" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B144" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="C144" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D144" t="str">
+        <x:v>761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="E144" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="145">
+      <x:c r="A145" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B145" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bab4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="C145" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D145" t="str">
+        <x:v>b4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="E145" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="146">
+      <x:c r="A146" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B146" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658badeb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="C146" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D146" t="str">
+        <x:v>deb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="E146" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="147">
+      <x:c r="A147" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B147" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bac39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="C147" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D147" t="str">
+        <x:v>c39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="E147" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="148">
+      <x:c r="A148" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B148" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bac39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="C148" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D148" t="str">
+        <x:v>c39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="E148" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="149">
+      <x:c r="A149" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B149" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba52022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="C149" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D149" t="str">
+        <x:v>52022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="E149" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="150">
+      <x:c r="A150" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B150" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba3a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="C150" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D150" t="str">
+        <x:v>3a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="E150" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="151">
+      <x:c r="A151" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B151" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba54787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="C151" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D151" t="str">
+        <x:v>54787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="E151" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="152">
+      <x:c r="A152" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B152" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba54787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="C152" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D152" t="str">
+        <x:v>54787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="E152" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="153">
+      <x:c r="A153" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B153" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bad1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="C153" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D153" t="str">
+        <x:v>d1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="E153" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="154">
+      <x:c r="A154" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B154" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bad1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="C154" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D154" t="str">
+        <x:v>d1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="E154" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155">
+      <x:c r="A155" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B155" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bae449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="C155" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D155" t="str">
+        <x:v>e449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="E155" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156">
+      <x:c r="A156" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B156" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658bae449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="C156" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D156" t="str">
+        <x:v>e449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="E156" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157">
+      <x:c r="A157" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B157" t="str">
+        <x:v>4cf300e2-1b35-41f4-88e3-713a387658ba416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="C157" t="str">
+        <x:v>1934291</x:v>
+      </x:c>
+      <x:c r="D157" t="str">
+        <x:v>416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="E157" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158">
+      <x:c r="A158" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B158" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62554787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="C158" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D158" t="str">
+        <x:v>54787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="E158" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159">
+      <x:c r="A159" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B159" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625c39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="C159" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D159" t="str">
+        <x:v> </x:v>
+      </x:c>
+      <x:c r="E159" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160">
+      <x:c r="A160" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B160" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6253a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="C160" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D160" t="str">
+        <x:v>3a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="E160" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="161">
+      <x:c r="A161" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B161" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62546f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="C161" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D161" t="str">
+        <x:v>46f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="E161" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="162">
+      <x:c r="A162" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B162" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625a294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="C162" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D162" t="str">
+        <x:v>a294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="E162" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="163">
+      <x:c r="A163" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B163" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625b4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="C163" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D163" t="str">
+        <x:v>b4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="E163" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="164">
+      <x:c r="A164" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B164" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62531bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="C164" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D164" t="str">
+        <x:v>31bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="E164" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="165">
+      <x:c r="A165" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B165" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62531bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="C165" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D165" t="str">
+        <x:v>31bd5344-dc5f-4eef-b1fe-4ef6aab5f2eb</x:v>
+      </x:c>
+      <x:c r="E165" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="166">
+      <x:c r="A166" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B166" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6258ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="C166" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D166" t="str">
+        <x:v>8ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="E166" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="167">
+      <x:c r="A167" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B167" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6258ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="C167" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D167" t="str">
+        <x:v>8ee2d2f2-a9f3-4f4c-84c3-b685092faf66</x:v>
+      </x:c>
+      <x:c r="E167" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="168">
+      <x:c r="A168" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B168" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625f0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="C168" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D168" t="str">
+        <x:v>f0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="E168" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="169">
+      <x:c r="A169" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B169" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625f0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="C169" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D169" t="str">
+        <x:v>f0b81127-6613-462a-a346-543b12ed5be6</x:v>
+      </x:c>
+      <x:c r="E169" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="170">
+      <x:c r="A170" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B170" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6259237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="C170" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D170" t="str">
+        <x:v>9237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="E170" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="171">
+      <x:c r="A171" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B171" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6259237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="C171" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D171" t="str">
+        <x:v>9237ff3d-d831-42c7-9187-dd8b8b236910</x:v>
+      </x:c>
+      <x:c r="E171" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="172">
+      <x:c r="A172" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B172" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625d1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="C172" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D172" t="str">
+        <x:v>d1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="E172" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="173">
+      <x:c r="A173" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B173" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625d1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="C173" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D173" t="str">
+        <x:v>d1659b6d-82f8-4446-940e-aa103c116ec0</x:v>
+      </x:c>
+      <x:c r="E173" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="174">
+      <x:c r="A174" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B174" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62554787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="C174" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D174" t="str">
+        <x:v>54787c0c-4678-48b9-a567-7cc5e69931ac</x:v>
+      </x:c>
+      <x:c r="E174" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="175">
+      <x:c r="A175" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B175" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625c39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="C175" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D175" t="str">
+        <x:v>c39e2c38-422d-447a-95bd-a7e34becc927</x:v>
+      </x:c>
+      <x:c r="E175" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="176">
+      <x:c r="A176" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B176" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6254c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="C176" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D176" t="str">
+        <x:v>4c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="E176" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="177">
+      <x:c r="A177" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B177" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6254c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="C177" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D177" t="str">
+        <x:v>4c517391-4b27-4b3f-97f8-c907a0cc22d2</x:v>
+      </x:c>
+      <x:c r="E177" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="178">
+      <x:c r="A178" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B178" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625e5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="C178" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D178" t="str">
+        <x:v>e5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="E178" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="179">
+      <x:c r="A179" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B179" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6253a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="C179" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D179" t="str">
+        <x:v>3a4766e9-a762-4b3d-a8be-fa98d43499f1</x:v>
+      </x:c>
+      <x:c r="E179" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="180">
+      <x:c r="A180" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B180" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62546f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="C180" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D180" t="str">
+        <x:v>46f41b89-be25-4773-93a6-89775ccf3a7f</x:v>
+      </x:c>
+      <x:c r="E180" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="181">
+      <x:c r="A181" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B181" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625a294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="C181" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D181" t="str">
+        <x:v>a294c5ea-be31-4bd4-90d9-678831f5356c</x:v>
+      </x:c>
+      <x:c r="E181" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="182">
+      <x:c r="A182" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B182" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625b4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="C182" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D182" t="str">
+        <x:v>b4c6113a-1d67-468d-a545-0feac00c43af</x:v>
+      </x:c>
+      <x:c r="E182" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="183">
+      <x:c r="A183" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B183" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62536dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="C183" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D183" t="str">
+        <x:v>36dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="E183" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="184">
+      <x:c r="A184" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B184" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62536dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="C184" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D184" t="str">
+        <x:v>36dd2013-8641-4239-8567-51060431629f</x:v>
+      </x:c>
+      <x:c r="E184" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="185">
+      <x:c r="A185" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B185" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6250d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="C185" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D185" t="str">
+        <x:v>0d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="E185" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="186">
+      <x:c r="A186" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B186" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6250d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="C186" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D186" t="str">
+        <x:v>0d14c4e8-424c-4208-8b48-665dffb359af</x:v>
+      </x:c>
+      <x:c r="E186" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="187">
+      <x:c r="A187" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B187" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="C187" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D187" t="str">
+        <x:v>416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="E187" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="188">
+      <x:c r="A188" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B188" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="C188" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D188" t="str">
+        <x:v>416e5764-ef23-4e9c-8810-2948a42a4dd0</x:v>
+      </x:c>
+      <x:c r="E188" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="189">
+      <x:c r="A189" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B189" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625deb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="C189" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D189" t="str">
+        <x:v>deb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="E189" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="190">
+      <x:c r="A190" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B190" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625deb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="C190" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D190" t="str">
+        <x:v>deb653f7-d4f8-47a7-848a-83ee64ddcd96</x:v>
+      </x:c>
+      <x:c r="E190" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="191">
+      <x:c r="A191" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B191" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6258ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="C191" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D191" t="str">
+        <x:v>8ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="E191" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="192">
+      <x:c r="A192" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B192" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6258ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="C192" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D192" t="str">
+        <x:v>8ce90744-4bc0-4e7c-b612-e6f05264120b</x:v>
+      </x:c>
+      <x:c r="E192" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="193">
+      <x:c r="A193" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B193" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625a6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="C193" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D193" t="str">
+        <x:v>a6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="E193" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="194">
+      <x:c r="A194" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B194" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625a6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="C194" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D194" t="str">
+        <x:v>a6a3daab-6e56-486b-9cfa-2038eafd36f3</x:v>
+      </x:c>
+      <x:c r="E194" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="195">
+      <x:c r="A195" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B195" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6253b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="C195" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D195" t="str">
+        <x:v>3b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="E195" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="196">
+      <x:c r="A196" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B196" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6253b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="C196" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D196" t="str">
+        <x:v>3b4ca3b3-7da4-46ea-833e-7547e56fa6ad</x:v>
+      </x:c>
+      <x:c r="E196" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="197">
+      <x:c r="A197" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B197" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62529b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="C197" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D197" t="str">
+        <x:v>29b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="E197" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="198">
+      <x:c r="A198" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B198" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62529b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="C198" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D198" t="str">
+        <x:v>29b1a97f-c5c0-48cf-af7e-117867f75ddf</x:v>
+      </x:c>
+      <x:c r="E198" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="199">
+      <x:c r="A199" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B199" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625dcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="C199" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D199" t="str">
+        <x:v>dcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="E199" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="200">
+      <x:c r="A200" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B200" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62552022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="C200" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D200" t="str">
+        <x:v>52022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="E200" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="201">
+      <x:c r="A201" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B201" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625e1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="C201" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D201" t="str">
+        <x:v>e1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="E201" t="str">
+        <x:v>yes</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="202">
+      <x:c r="A202" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B202" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6259be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="C202" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D202" t="str">
+        <x:v>9be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="E202" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="203">
+      <x:c r="A203" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B203" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6259be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="C203" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D203" t="str">
+        <x:v>9be167e0-2c89-4386-b02a-2468c2c7f2bc</x:v>
+      </x:c>
+      <x:c r="E203" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="204">
+      <x:c r="A204" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B204" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625e449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="C204" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D204" t="str">
+        <x:v>e449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="E204" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="205">
+      <x:c r="A205" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B205" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625e449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="C205" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D205" t="str">
+        <x:v>e449c9c7-802c-47ec-9cf8-5a173d45579b</x:v>
+      </x:c>
+      <x:c r="E205" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="206">
+      <x:c r="A206" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B206" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625e5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="C206" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D206" t="str">
+        <x:v>e5615e1a-2ded-45f1-98af-2f10c96caaaf</x:v>
+      </x:c>
+      <x:c r="E206" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="207">
+      <x:c r="A207" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B207" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625d5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="C207" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D207" t="str">
+        <x:v>d5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="E207" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="208">
+      <x:c r="A208" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B208" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="C208" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D208" t="str">
+        <x:v>761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="E208" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="209">
+      <x:c r="A209" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B209" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62552022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="C209" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D209" t="str">
+        <x:v>52022723-15f9-4012-9e22-1b86e161b05b</x:v>
+      </x:c>
+      <x:c r="E209" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="210">
+      <x:c r="A210" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B210" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6255b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="C210" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D210" t="str">
+        <x:v>5b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="E210" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="211">
+      <x:c r="A211" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B211" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6255b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="C211" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D211" t="str">
+        <x:v>5b20e08f-26e4-4cf8-81ac-d60f629f106b</x:v>
+      </x:c>
+      <x:c r="E211" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="212">
+      <x:c r="A212" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B212" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62575357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="C212" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D212" t="str">
+        <x:v>75357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="E212" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="213">
+      <x:c r="A213" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B213" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c62575357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="C213" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D213" t="str">
+        <x:v>75357e44-832c-4882-ba02-80425a673fca</x:v>
+      </x:c>
+      <x:c r="E213" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="214">
+      <x:c r="A214" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B214" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625e1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="C214" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D214" t="str">
+        <x:v>e1dcbd79-5188-41b5-95c0-6dc8ea246a09</x:v>
+      </x:c>
+      <x:c r="E214" t="str">
+        <x:v>yes</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="215">
+      <x:c r="A215" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B215" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625dcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="C215" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D215" t="str">
+        <x:v>dcd05c83-7c18-49fd-8d73-69a3fad71e8a</x:v>
+      </x:c>
+      <x:c r="E215" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="216">
+      <x:c r="A216" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B216" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6251e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="C216" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D216" t="str">
+        <x:v>1e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="E216" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="217">
+      <x:c r="A217" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B217" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c6251e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="C217" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D217" t="str">
+        <x:v>1e37e0b7-9c94-420f-97c6-b5ea8ef60212</x:v>
+      </x:c>
+      <x:c r="E217" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="218">
+      <x:c r="A218" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B218" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625d5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="C218" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D218" t="str">
+        <x:v>d5644e4e-e4a3-4718-8b47-eefeb37624c5</x:v>
+      </x:c>
+      <x:c r="E218" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="219">
+      <x:c r="A219" t="str">
+        <x:v>update</x:v>
+      </x:c>
+      <x:c r="B219" t="str">
+        <x:v>9762d835-7fe4-4769-a096-9866c9c9c625761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="C219" t="str">
+        <x:v>1934293</x:v>
+      </x:c>
+      <x:c r="D219" t="str">
+        <x:v>761ebc1a-2d09-4588-bddd-c18cb87198cc</x:v>
+      </x:c>
+      <x:c r="E219" t="str">
+        <x:v>no</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
 </x:worksheet>
 </file>
</xml_diff>